<commit_message>
wrap text and auto open
</commit_message>
<xml_diff>
--- a/File/jobs.xlsx
+++ b/File/jobs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Title</t>
   </si>
@@ -43,36 +43,6 @@
     <t>AWS DevOps/Linux Admin</t>
   </si>
   <si>
-    <t>React Developer</t>
-  </si>
-  <si>
-    <t>UI Developer</t>
-  </si>
-  <si>
-    <t>QA Engineer</t>
-  </si>
-  <si>
-    <t>DevOps Engineer</t>
-  </si>
-  <si>
-    <t>Java Developer (Account Managem…</t>
-  </si>
-  <si>
-    <t>API Developer (MuleSoft)</t>
-  </si>
-  <si>
-    <t>ETL Developer (Informatica)</t>
-  </si>
-  <si>
-    <t>ETL Developer (Talend)</t>
-  </si>
-  <si>
-    <t>Software Test Engineer</t>
-  </si>
-  <si>
-    <t>Product Manager</t>
-  </si>
-  <si>
     <t>CloudHero</t>
   </si>
   <si>
@@ -82,15 +52,6 @@
     <t>Verisk Nepal</t>
   </si>
   <si>
-    <t>Smart Data Solution</t>
-  </si>
-  <si>
-    <t>BI-SOLUTIONS</t>
-  </si>
-  <si>
-    <t>WhiteHat Engineering Inc.</t>
-  </si>
-  <si>
     <t>Communication,Devops,Cloud Computing,Linux,Kubernetes,</t>
   </si>
   <si>
@@ -103,24 +64,6 @@
     <t>Devops,Aws,</t>
   </si>
   <si>
-    <t>Interpersonal,Management,Communication,Html,</t>
-  </si>
-  <si>
-    <t>Interpersonal,Communication,Technical,</t>
-  </si>
-  <si>
-    <t>Interpersonal,Management,Communication,</t>
-  </si>
-  <si>
-    <t>Html,Jquery,Javascript,Java And Object Oriented Programming,</t>
-  </si>
-  <si>
-    <t>Mulesoft,</t>
-  </si>
-  <si>
-    <t>Node.Js,Ror,Java,Python,</t>
-  </si>
-  <si>
     <t>https://merojob.com/senior-devops-engineer-11/</t>
   </si>
   <si>
@@ -134,36 +77,6 @@
   </si>
   <si>
     <t>https://merojob.com/aws-devopslinux-admin-3/</t>
-  </si>
-  <si>
-    <t>https://merojob.com/react-developer-55/</t>
-  </si>
-  <si>
-    <t>https://merojob.com/ui-developer-8/</t>
-  </si>
-  <si>
-    <t>https://merojob.com/qa-engineer-74/</t>
-  </si>
-  <si>
-    <t>https://merojob.com/devops-engineer-45/</t>
-  </si>
-  <si>
-    <t>https://merojob.com/java-developer-173/</t>
-  </si>
-  <si>
-    <t>https://merojob.com/api-developer/</t>
-  </si>
-  <si>
-    <t>https://merojob.com/etl-developer-informatica/</t>
-  </si>
-  <si>
-    <t>https://merojob.com/etl-developer-talend/</t>
-  </si>
-  <si>
-    <t>https://merojob.com/software-test-engineer-19/</t>
-  </si>
-  <si>
-    <t>https://merojob.com/product-manager-50/</t>
   </si>
 </sst>
 </file>
@@ -537,7 +450,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -565,13 +478,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -579,10 +492,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -590,13 +503,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -604,13 +517,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -618,144 +531,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -765,16 +547,6 @@
     <hyperlink ref="D4" r:id="rId3"/>
     <hyperlink ref="D5" r:id="rId4"/>
     <hyperlink ref="D6" r:id="rId5"/>
-    <hyperlink ref="D7" r:id="rId6"/>
-    <hyperlink ref="D8" r:id="rId7"/>
-    <hyperlink ref="D9" r:id="rId8"/>
-    <hyperlink ref="D10" r:id="rId9"/>
-    <hyperlink ref="D11" r:id="rId10"/>
-    <hyperlink ref="D12" r:id="rId11"/>
-    <hyperlink ref="D13" r:id="rId12"/>
-    <hyperlink ref="D14" r:id="rId13"/>
-    <hyperlink ref="D15" r:id="rId14"/>
-    <hyperlink ref="D16" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>